<commit_message>
used STAC to load CHIRPS data
</commit_message>
<xml_diff>
--- a/data/smartfarmer_contacts.xlsx
+++ b/data/smartfarmer_contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\ownCloud2\Projects\2021\Digital Earth Africa_ Innovation challenge\Impelemntation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5055BF05-AAA2-4188-87E9-4280E9AE6A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38419D93-6061-423D-8E52-13BE166C89DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,33 @@
   </si>
   <si>
     <t>03.11.2021</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>0.735884</t>
+  </si>
+  <si>
+    <t>34.5833</t>
+  </si>
+  <si>
+    <t>0.055216</t>
+  </si>
+  <si>
+    <t>34.2770</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>H84</t>
+  </si>
+  <si>
+    <t>SC Saga</t>
   </si>
 </sst>
 </file>
@@ -101,11 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -386,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,9 +425,10 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="18.08984375" customWidth="1"/>
     <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -412,8 +441,17 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -426,8 +464,17 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -439,6 +486,15 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>